<commit_message>
add UDS Form A4
</commit_message>
<xml_diff>
--- a/WIP__uds3_ift_matches.xlsx
+++ b/WIP__uds3_ift_matches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ldmay/Box Sync/Documents/MADC_Data_Unification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A695D10F-F4A3-A540-853D-088FE3D553A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DABCDDC-77DF-5841-9F41-BA2D3C4968E8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19180" yWindow="460" windowWidth="19200" windowHeight="23540" xr2:uid="{076664BD-647D-FA4F-B94B-D41FA05C105D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2141" uniqueCount="1084">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="1243">
   <si>
     <t>ivp_a1</t>
   </si>
@@ -3282,6 +3282,483 @@
   </si>
   <si>
     <t>ivp_tvp_match</t>
+  </si>
+  <si>
+    <t>anymeds</t>
+  </si>
+  <si>
+    <t>drugid_1</t>
+  </si>
+  <si>
+    <t>drugid_2</t>
+  </si>
+  <si>
+    <t>drugid_3</t>
+  </si>
+  <si>
+    <t>drugid_4</t>
+  </si>
+  <si>
+    <t>drugid_5</t>
+  </si>
+  <si>
+    <t>drugid_6</t>
+  </si>
+  <si>
+    <t>drugid_7</t>
+  </si>
+  <si>
+    <t>drugid_8</t>
+  </si>
+  <si>
+    <t>drugid_9</t>
+  </si>
+  <si>
+    <t>drugid_10</t>
+  </si>
+  <si>
+    <t>drugid_11</t>
+  </si>
+  <si>
+    <t>drugid_12</t>
+  </si>
+  <si>
+    <t>drugid_13</t>
+  </si>
+  <si>
+    <t>drugid_14</t>
+  </si>
+  <si>
+    <t>drugid_15</t>
+  </si>
+  <si>
+    <t>drugid_16</t>
+  </si>
+  <si>
+    <t>drugid_17</t>
+  </si>
+  <si>
+    <t>drugid_18</t>
+  </si>
+  <si>
+    <t>drugid_19</t>
+  </si>
+  <si>
+    <t>drugid_20</t>
+  </si>
+  <si>
+    <t>drugid_21</t>
+  </si>
+  <si>
+    <t>drugid_22</t>
+  </si>
+  <si>
+    <t>drugid_23</t>
+  </si>
+  <si>
+    <t>drugid_24</t>
+  </si>
+  <si>
+    <t>drugid_25</t>
+  </si>
+  <si>
+    <t>drugid_26</t>
+  </si>
+  <si>
+    <t>drugid_27</t>
+  </si>
+  <si>
+    <t>drugid_28</t>
+  </si>
+  <si>
+    <t>drugid_29</t>
+  </si>
+  <si>
+    <t>drugid_30</t>
+  </si>
+  <si>
+    <t>drugid_31</t>
+  </si>
+  <si>
+    <t>drugid_32</t>
+  </si>
+  <si>
+    <t>drugid_33</t>
+  </si>
+  <si>
+    <t>drugid_34</t>
+  </si>
+  <si>
+    <t>drugid_35</t>
+  </si>
+  <si>
+    <t>drugid_36</t>
+  </si>
+  <si>
+    <t>drugid_37</t>
+  </si>
+  <si>
+    <t>drugid_38</t>
+  </si>
+  <si>
+    <t>drugid_39</t>
+  </si>
+  <si>
+    <t>drugid_40</t>
+  </si>
+  <si>
+    <t>drugid_41</t>
+  </si>
+  <si>
+    <t>drugid_42</t>
+  </si>
+  <si>
+    <t>drugid_43</t>
+  </si>
+  <si>
+    <t>drugid_44</t>
+  </si>
+  <si>
+    <t>drugid_45</t>
+  </si>
+  <si>
+    <t>drugid_46</t>
+  </si>
+  <si>
+    <t>drugid_47</t>
+  </si>
+  <si>
+    <t>drugid_48</t>
+  </si>
+  <si>
+    <t>drugid_49</t>
+  </si>
+  <si>
+    <t>drugid_50</t>
+  </si>
+  <si>
+    <t>ivp_a4_complete</t>
+  </si>
+  <si>
+    <t>ivp_a4</t>
+  </si>
+  <si>
+    <t>fu_anymeds</t>
+  </si>
+  <si>
+    <t>fu_drugid_1</t>
+  </si>
+  <si>
+    <t>fu_drugid_2</t>
+  </si>
+  <si>
+    <t>fu_drugid_3</t>
+  </si>
+  <si>
+    <t>fu_drugid_4</t>
+  </si>
+  <si>
+    <t>fu_drugid_5</t>
+  </si>
+  <si>
+    <t>fu_drugid_6</t>
+  </si>
+  <si>
+    <t>fu_drugid_7</t>
+  </si>
+  <si>
+    <t>fu_drugid_8</t>
+  </si>
+  <si>
+    <t>fu_drugid_9</t>
+  </si>
+  <si>
+    <t>fu_drugid_10</t>
+  </si>
+  <si>
+    <t>fu_drugid_11</t>
+  </si>
+  <si>
+    <t>fu_drugid_12</t>
+  </si>
+  <si>
+    <t>fu_drugid_13</t>
+  </si>
+  <si>
+    <t>fu_drugid_14</t>
+  </si>
+  <si>
+    <t>fu_drugid_15</t>
+  </si>
+  <si>
+    <t>fu_drugid_16</t>
+  </si>
+  <si>
+    <t>fu_drugid_17</t>
+  </si>
+  <si>
+    <t>fu_drugid_18</t>
+  </si>
+  <si>
+    <t>fu_drugid_19</t>
+  </si>
+  <si>
+    <t>fu_drugid_20</t>
+  </si>
+  <si>
+    <t>fu_drugid_21</t>
+  </si>
+  <si>
+    <t>fu_drugid_22</t>
+  </si>
+  <si>
+    <t>fu_drugid_23</t>
+  </si>
+  <si>
+    <t>fu_drugid_24</t>
+  </si>
+  <si>
+    <t>fu_drugid_25</t>
+  </si>
+  <si>
+    <t>fu_drugid_26</t>
+  </si>
+  <si>
+    <t>fu_drugid_27</t>
+  </si>
+  <si>
+    <t>fu_drugid_28</t>
+  </si>
+  <si>
+    <t>fu_drugid_29</t>
+  </si>
+  <si>
+    <t>fu_drugid_30</t>
+  </si>
+  <si>
+    <t>fu_drugid_31</t>
+  </si>
+  <si>
+    <t>fu_drugid_32</t>
+  </si>
+  <si>
+    <t>fu_drugid_33</t>
+  </si>
+  <si>
+    <t>fu_drugid_34</t>
+  </si>
+  <si>
+    <t>fu_drugid_35</t>
+  </si>
+  <si>
+    <t>fu_drugid_36</t>
+  </si>
+  <si>
+    <t>fu_drugid_37</t>
+  </si>
+  <si>
+    <t>fu_drugid_38</t>
+  </si>
+  <si>
+    <t>fu_drugid_39</t>
+  </si>
+  <si>
+    <t>fu_drugid_40</t>
+  </si>
+  <si>
+    <t>fu_drugid_41</t>
+  </si>
+  <si>
+    <t>fu_drugid_42</t>
+  </si>
+  <si>
+    <t>fu_drugid_43</t>
+  </si>
+  <si>
+    <t>fu_drugid_44</t>
+  </si>
+  <si>
+    <t>fu_drugid_45</t>
+  </si>
+  <si>
+    <t>fu_drugid_46</t>
+  </si>
+  <si>
+    <t>fu_drugid_47</t>
+  </si>
+  <si>
+    <t>fu_drugid_48</t>
+  </si>
+  <si>
+    <t>fu_drugid_49</t>
+  </si>
+  <si>
+    <t>fu_drugid_50</t>
+  </si>
+  <si>
+    <t>fvp_a4_complete</t>
+  </si>
+  <si>
+    <t>fvp_a4</t>
+  </si>
+  <si>
+    <t>tvp_anymeds</t>
+  </si>
+  <si>
+    <t>tele_drugid_1</t>
+  </si>
+  <si>
+    <t>tele_drugid_2</t>
+  </si>
+  <si>
+    <t>tele_drugid_3</t>
+  </si>
+  <si>
+    <t>tele_drugid_4</t>
+  </si>
+  <si>
+    <t>tele_drugid_5</t>
+  </si>
+  <si>
+    <t>tele_drugid_6</t>
+  </si>
+  <si>
+    <t>tele_drugid_7</t>
+  </si>
+  <si>
+    <t>tele_drugid_8</t>
+  </si>
+  <si>
+    <t>tele_drugid_9</t>
+  </si>
+  <si>
+    <t>tele_drugid_10</t>
+  </si>
+  <si>
+    <t>tele_drugid_11</t>
+  </si>
+  <si>
+    <t>tele_drugid_12</t>
+  </si>
+  <si>
+    <t>tele_drugid_13</t>
+  </si>
+  <si>
+    <t>tele_drugid_14</t>
+  </si>
+  <si>
+    <t>tele_drugid_15</t>
+  </si>
+  <si>
+    <t>tele_drugid_16</t>
+  </si>
+  <si>
+    <t>tele_drugid_17</t>
+  </si>
+  <si>
+    <t>tele_drugid_18</t>
+  </si>
+  <si>
+    <t>tele_drugid_19</t>
+  </si>
+  <si>
+    <t>tele_drugid_20</t>
+  </si>
+  <si>
+    <t>tele_drugid_21</t>
+  </si>
+  <si>
+    <t>tele_drugid_22</t>
+  </si>
+  <si>
+    <t>tele_drugid_23</t>
+  </si>
+  <si>
+    <t>tele_drugid_24</t>
+  </si>
+  <si>
+    <t>tele_drugid_25</t>
+  </si>
+  <si>
+    <t>tele_drugid_26</t>
+  </si>
+  <si>
+    <t>tele_drugid_27</t>
+  </si>
+  <si>
+    <t>tele_drugid_28</t>
+  </si>
+  <si>
+    <t>tele_drugid_29</t>
+  </si>
+  <si>
+    <t>tele_drugid_30</t>
+  </si>
+  <si>
+    <t>tele_drugid_31</t>
+  </si>
+  <si>
+    <t>tele_drugid_32</t>
+  </si>
+  <si>
+    <t>tele_drugid_33</t>
+  </si>
+  <si>
+    <t>tele_drugid_34</t>
+  </si>
+  <si>
+    <t>tele_drugid_35</t>
+  </si>
+  <si>
+    <t>tele_drugid_36</t>
+  </si>
+  <si>
+    <t>tele_drugid_37</t>
+  </si>
+  <si>
+    <t>tele_drugid_38</t>
+  </si>
+  <si>
+    <t>tele_drugid_39</t>
+  </si>
+  <si>
+    <t>tele_drugid_40</t>
+  </si>
+  <si>
+    <t>tele_drugid_41</t>
+  </si>
+  <si>
+    <t>tele_drugid_42</t>
+  </si>
+  <si>
+    <t>tele_drugid_43</t>
+  </si>
+  <si>
+    <t>tele_drugid_44</t>
+  </si>
+  <si>
+    <t>tele_drugid_45</t>
+  </si>
+  <si>
+    <t>tele_drugid_46</t>
+  </si>
+  <si>
+    <t>tele_drugid_47</t>
+  </si>
+  <si>
+    <t>tele_drugid_48</t>
+  </si>
+  <si>
+    <t>tele_drugid_49</t>
+  </si>
+  <si>
+    <t>tele_drugid_50</t>
+  </si>
+  <si>
+    <t>tvp_a4_complete</t>
+  </si>
+  <si>
+    <t>tvp_a4</t>
   </si>
 </sst>
 </file>
@@ -3332,7 +3809,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3673,11 +4160,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCC9BF6-0E02-034A-99C2-203518C15656}">
-  <dimension ref="A1:H372"/>
+  <dimension ref="A1:H424"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H373" sqref="H373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12461,7 +12948,7 @@
         <v>717</v>
       </c>
       <c r="D323" t="b">
-        <f t="shared" ref="D323:D372" si="10">IF(NOT(ISBLANK(C323)),A323=REPLACE(C323,1,3,""),"")</f>
+        <f t="shared" ref="D323:D386" si="10">IF(NOT(ISBLANK(C323)),A323=REPLACE(C323,1,3,""),"")</f>
         <v>1</v>
       </c>
       <c r="E323" t="s">
@@ -12474,7 +12961,7 @@
         <v>1080</v>
       </c>
       <c r="H323" t="b">
-        <f t="shared" ref="H323:H372" si="11">IF(NOT(ISBLANK(F323)),A323=REPLACE(F323,1,5,""),"")</f>
+        <f t="shared" ref="H323:H386" si="11">IF(NOT(ISBLANK(F323)),A323=REPLACE(F323,1,5,""),"")</f>
         <v>1</v>
       </c>
     </row>
@@ -13738,7 +14225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C369" t="s">
         <v>446</v>
       </c>
@@ -13760,7 +14247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C370" t="s">
         <v>459</v>
       </c>
@@ -13782,7 +14269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C371" t="s">
         <v>477</v>
       </c>
@@ -13804,7 +14291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C372" t="s">
         <v>640</v>
       </c>
@@ -13826,13 +14313,1479 @@
         <v>0</v>
       </c>
     </row>
+    <row r="373" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A373" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B373" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C373" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D373" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E373" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F373" t="s">
+        <v>1190</v>
+      </c>
+      <c r="G373" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H373" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A374" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B374" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C374" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D374" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E374" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F374" t="s">
+        <v>1191</v>
+      </c>
+      <c r="G374" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H374" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A375" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B375" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C375" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D375" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E375" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F375" t="s">
+        <v>1192</v>
+      </c>
+      <c r="G375" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H375" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A376" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B376" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C376" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D376" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E376" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F376" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G376" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H376" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A377" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B377" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C377" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D377" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E377" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F377" t="s">
+        <v>1194</v>
+      </c>
+      <c r="G377" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H377" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="378" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A378" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B378" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C378" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D378" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E378" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F378" t="s">
+        <v>1195</v>
+      </c>
+      <c r="G378" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H378" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="379" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A379" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B379" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C379" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D379" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E379" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F379" t="s">
+        <v>1196</v>
+      </c>
+      <c r="G379" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H379" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A380" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B380" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C380" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D380" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E380" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F380" t="s">
+        <v>1197</v>
+      </c>
+      <c r="G380" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H380" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A381" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B381" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C381" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D381" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E381" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F381" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G381" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H381" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="382" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A382" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B382" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C382" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D382" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E382" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F382" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G382" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H382" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A383" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B383" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C383" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D383" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E383" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F383" t="s">
+        <v>1200</v>
+      </c>
+      <c r="G383" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H383" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A384" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B384" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C384" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D384" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E384" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F384" t="s">
+        <v>1201</v>
+      </c>
+      <c r="G384" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H384" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A385" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B385" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C385" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D385" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E385" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F385" t="s">
+        <v>1202</v>
+      </c>
+      <c r="G385" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H385" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A386" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B386" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C386" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D386" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E386" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F386" t="s">
+        <v>1203</v>
+      </c>
+      <c r="G386" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H386" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A387" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B387" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C387" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D387" t="b">
+        <f t="shared" ref="D387:D424" si="12">IF(NOT(ISBLANK(C387)),A387=REPLACE(C387,1,3,""),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E387" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F387" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G387" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H387" t="b">
+        <f t="shared" ref="H387:H424" si="13">IF(NOT(ISBLANK(F387)),A387=REPLACE(F387,1,5,""),"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="388" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A388" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B388" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C388" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D388" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E388" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F388" t="s">
+        <v>1205</v>
+      </c>
+      <c r="G388" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H388" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A389" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B389" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C389" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D389" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E389" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F389" t="s">
+        <v>1206</v>
+      </c>
+      <c r="G389" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H389" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A390" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B390" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C390" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D390" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E390" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F390" t="s">
+        <v>1207</v>
+      </c>
+      <c r="G390" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H390" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A391" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B391" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C391" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D391" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E391" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F391" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G391" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H391" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="392" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A392" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B392" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C392" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D392" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E392" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F392" t="s">
+        <v>1209</v>
+      </c>
+      <c r="G392" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H392" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A393" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B393" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C393" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D393" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E393" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F393" t="s">
+        <v>1210</v>
+      </c>
+      <c r="G393" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H393" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="394" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A394" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B394" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C394" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D394" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E394" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F394" t="s">
+        <v>1211</v>
+      </c>
+      <c r="G394" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H394" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A395" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B395" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C395" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D395" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E395" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F395" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G395" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H395" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A396" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B396" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C396" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D396" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E396" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F396" t="s">
+        <v>1213</v>
+      </c>
+      <c r="G396" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H396" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="397" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A397" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B397" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C397" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D397" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E397" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F397" t="s">
+        <v>1214</v>
+      </c>
+      <c r="G397" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H397" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A398" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B398" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C398" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D398" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E398" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F398" t="s">
+        <v>1215</v>
+      </c>
+      <c r="G398" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H398" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A399" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B399" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C399" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D399" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E399" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F399" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G399" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H399" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A400" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B400" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C400" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D400" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E400" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F400" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G400" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H400" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A401" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B401" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C401" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D401" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E401" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F401" t="s">
+        <v>1218</v>
+      </c>
+      <c r="G401" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H401" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A402" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B402" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C402" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D402" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E402" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F402" t="s">
+        <v>1219</v>
+      </c>
+      <c r="G402" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H402" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A403" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B403" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C403" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D403" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E403" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F403" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G403" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H403" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A404" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B404" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C404" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D404" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E404" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F404" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G404" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H404" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A405" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B405" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C405" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D405" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E405" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F405" t="s">
+        <v>1222</v>
+      </c>
+      <c r="G405" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H405" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="406" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A406" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B406" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C406" t="s">
+        <v>1170</v>
+      </c>
+      <c r="D406" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E406" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F406" t="s">
+        <v>1223</v>
+      </c>
+      <c r="G406" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H406" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="407" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A407" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B407" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C407" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D407" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E407" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F407" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G407" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H407" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A408" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B408" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C408" t="s">
+        <v>1172</v>
+      </c>
+      <c r="D408" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E408" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F408" t="s">
+        <v>1225</v>
+      </c>
+      <c r="G408" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H408" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="409" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A409" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B409" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C409" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D409" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E409" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F409" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G409" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H409" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="410" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A410" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B410" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C410" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D410" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E410" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F410" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G410" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H410" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="411" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A411" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B411" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C411" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D411" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E411" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F411" t="s">
+        <v>1228</v>
+      </c>
+      <c r="G411" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H411" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="412" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A412" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B412" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C412" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D412" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E412" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F412" t="s">
+        <v>1229</v>
+      </c>
+      <c r="G412" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H412" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="413" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A413" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B413" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C413" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D413" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E413" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F413" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G413" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H413" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="414" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A414" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B414" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C414" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D414" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E414" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F414" t="s">
+        <v>1231</v>
+      </c>
+      <c r="G414" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H414" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="415" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A415" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B415" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C415" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D415" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E415" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F415" t="s">
+        <v>1232</v>
+      </c>
+      <c r="G415" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H415" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A416" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B416" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C416" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D416" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E416" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F416" t="s">
+        <v>1233</v>
+      </c>
+      <c r="G416" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H416" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="417" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A417" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B417" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C417" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D417" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E417" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F417" t="s">
+        <v>1234</v>
+      </c>
+      <c r="G417" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H417" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="418" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A418" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B418" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C418" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D418" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E418" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F418" t="s">
+        <v>1235</v>
+      </c>
+      <c r="G418" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H418" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="419" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A419" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B419" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C419" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D419" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E419" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F419" t="s">
+        <v>1236</v>
+      </c>
+      <c r="G419" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H419" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A420" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B420" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C420" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D420" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E420" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F420" t="s">
+        <v>1237</v>
+      </c>
+      <c r="G420" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H420" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A421" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B421" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C421" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D421" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E421" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F421" t="s">
+        <v>1238</v>
+      </c>
+      <c r="G421" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H421" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A422" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B422" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C422" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D422" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E422" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F422" t="s">
+        <v>1239</v>
+      </c>
+      <c r="G422" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H422" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A423" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B423" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C423" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D423" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E423" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F423" t="s">
+        <v>1240</v>
+      </c>
+      <c r="G423" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H423" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A424" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B424" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C424" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D424" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E424" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F424" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G424" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H424" t="b">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D1:D1048576 E373 E376 E379 E382 E385 E388 E391 E394 E397 E400 E403 E406 E409 E412 E415 E418 E421 E424">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E374 E377 E380 E383 E386 E389 E392 E395 E398 E401 E404 E407 E410 E413 E416 E419 E422">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
+  <conditionalFormatting sqref="E375 E378 E381 E384 E387 E390 E393 E396 E399 E402 E405 E408 E411 E414 E417 E420 E423">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>

</xml_diff>

<commit_message>
add UDS Form A5
</commit_message>
<xml_diff>
--- a/WIP__uds3_ift_matches.xlsx
+++ b/WIP__uds3_ift_matches.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ldmay/Box Sync/Documents/MADC_Data_Unification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DABCDDC-77DF-5841-9F41-BA2D3C4968E8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C821789E-2B23-D944-A902-237CFA80B4D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19180" yWindow="460" windowWidth="19200" windowHeight="23540" xr2:uid="{076664BD-647D-FA4F-B94B-D41FA05C105D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="1243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2729" uniqueCount="1383">
   <si>
     <t>ivp_a1</t>
   </si>
@@ -3759,6 +3759,426 @@
   </si>
   <si>
     <t>tvp_a4</t>
+  </si>
+  <si>
+    <t>tobac30</t>
+  </si>
+  <si>
+    <t>tobac100</t>
+  </si>
+  <si>
+    <t>smokyrs</t>
+  </si>
+  <si>
+    <t>packsper</t>
+  </si>
+  <si>
+    <t>quitsmok</t>
+  </si>
+  <si>
+    <t>alcoccas</t>
+  </si>
+  <si>
+    <t>alcfreq</t>
+  </si>
+  <si>
+    <t>cvhatt</t>
+  </si>
+  <si>
+    <t>hattmult</t>
+  </si>
+  <si>
+    <t>hattyear</t>
+  </si>
+  <si>
+    <t>cvafib</t>
+  </si>
+  <si>
+    <t>cvangio</t>
+  </si>
+  <si>
+    <t>cvbypass</t>
+  </si>
+  <si>
+    <t>cvpacdef</t>
+  </si>
+  <si>
+    <t>cvchf</t>
+  </si>
+  <si>
+    <t>cvangina</t>
+  </si>
+  <si>
+    <t>cvhvalve</t>
+  </si>
+  <si>
+    <t>cvothr</t>
+  </si>
+  <si>
+    <t>cvothrx</t>
+  </si>
+  <si>
+    <t>cbstroke</t>
+  </si>
+  <si>
+    <t>strokmul</t>
+  </si>
+  <si>
+    <t>strokyr</t>
+  </si>
+  <si>
+    <t>cbtia</t>
+  </si>
+  <si>
+    <t>tiamult</t>
+  </si>
+  <si>
+    <t>tiayear</t>
+  </si>
+  <si>
+    <t>pd</t>
+  </si>
+  <si>
+    <t>pdyr</t>
+  </si>
+  <si>
+    <t>pdothr</t>
+  </si>
+  <si>
+    <t>pdothryr</t>
+  </si>
+  <si>
+    <t>seizures</t>
+  </si>
+  <si>
+    <t>tbi</t>
+  </si>
+  <si>
+    <t>tbibrief</t>
+  </si>
+  <si>
+    <t>tbiexten</t>
+  </si>
+  <si>
+    <t>tbiwolos</t>
+  </si>
+  <si>
+    <t>tbiyear</t>
+  </si>
+  <si>
+    <t>diabetes</t>
+  </si>
+  <si>
+    <t>diabtype</t>
+  </si>
+  <si>
+    <t>hyperten</t>
+  </si>
+  <si>
+    <t>hypercho</t>
+  </si>
+  <si>
+    <t>b12def</t>
+  </si>
+  <si>
+    <t>thyroid</t>
+  </si>
+  <si>
+    <t>arthrit</t>
+  </si>
+  <si>
+    <t>arthtype</t>
+  </si>
+  <si>
+    <t>arthtypx</t>
+  </si>
+  <si>
+    <t>arthupex</t>
+  </si>
+  <si>
+    <t>arthloex</t>
+  </si>
+  <si>
+    <t>arthspin</t>
+  </si>
+  <si>
+    <t>arthunk</t>
+  </si>
+  <si>
+    <t>incontu</t>
+  </si>
+  <si>
+    <t>incontf</t>
+  </si>
+  <si>
+    <t>apnea</t>
+  </si>
+  <si>
+    <t>rbd</t>
+  </si>
+  <si>
+    <t>insomn</t>
+  </si>
+  <si>
+    <t>othsleep</t>
+  </si>
+  <si>
+    <t>othsleex</t>
+  </si>
+  <si>
+    <t>alcohol</t>
+  </si>
+  <si>
+    <t>abusothr</t>
+  </si>
+  <si>
+    <t>abusx</t>
+  </si>
+  <si>
+    <t>ptsd</t>
+  </si>
+  <si>
+    <t>bipolar</t>
+  </si>
+  <si>
+    <t>schiz</t>
+  </si>
+  <si>
+    <t>dep2yrs</t>
+  </si>
+  <si>
+    <t>depothr</t>
+  </si>
+  <si>
+    <t>anxiety</t>
+  </si>
+  <si>
+    <t>ocd</t>
+  </si>
+  <si>
+    <t>npsydev</t>
+  </si>
+  <si>
+    <t>psycdis</t>
+  </si>
+  <si>
+    <t>psycdisx</t>
+  </si>
+  <si>
+    <t>ivp_a5_complete</t>
+  </si>
+  <si>
+    <t>ivp_a5</t>
+  </si>
+  <si>
+    <t>fu_tobac30</t>
+  </si>
+  <si>
+    <t>fu_tobac100</t>
+  </si>
+  <si>
+    <t>fu_smokyrs</t>
+  </si>
+  <si>
+    <t>fu_packsper</t>
+  </si>
+  <si>
+    <t>fu_quitsmok</t>
+  </si>
+  <si>
+    <t>fu_alcoccas</t>
+  </si>
+  <si>
+    <t>fu_alcfreq</t>
+  </si>
+  <si>
+    <t>fu_cvhatt</t>
+  </si>
+  <si>
+    <t>fu_hattmult</t>
+  </si>
+  <si>
+    <t>fu_hattyear</t>
+  </si>
+  <si>
+    <t>fu_cvafib</t>
+  </si>
+  <si>
+    <t>fu_cvangio</t>
+  </si>
+  <si>
+    <t>fu_cvbypass</t>
+  </si>
+  <si>
+    <t>fu_cvpacdef</t>
+  </si>
+  <si>
+    <t>fu_cvchf</t>
+  </si>
+  <si>
+    <t>fu_cvangina</t>
+  </si>
+  <si>
+    <t>fu_cvhvalve</t>
+  </si>
+  <si>
+    <t>fu_cvothr</t>
+  </si>
+  <si>
+    <t>fu_cvothrx</t>
+  </si>
+  <si>
+    <t>fu_cbstroke</t>
+  </si>
+  <si>
+    <t>fu_strokmul</t>
+  </si>
+  <si>
+    <t>fu_strokyr</t>
+  </si>
+  <si>
+    <t>fu_cbtia</t>
+  </si>
+  <si>
+    <t>fu_tiamult</t>
+  </si>
+  <si>
+    <t>fu_tiayear</t>
+  </si>
+  <si>
+    <t>fu_pd</t>
+  </si>
+  <si>
+    <t>fu_pdyr</t>
+  </si>
+  <si>
+    <t>fu_pdothr</t>
+  </si>
+  <si>
+    <t>fu_pdothryr</t>
+  </si>
+  <si>
+    <t>fu_seizures</t>
+  </si>
+  <si>
+    <t>fu_tbi</t>
+  </si>
+  <si>
+    <t>fu_tbibrief</t>
+  </si>
+  <si>
+    <t>fu_tbiexten</t>
+  </si>
+  <si>
+    <t>fu_tbiwolos</t>
+  </si>
+  <si>
+    <t>fu_tbiyear</t>
+  </si>
+  <si>
+    <t>fu_diabetes</t>
+  </si>
+  <si>
+    <t>fu_diabtype</t>
+  </si>
+  <si>
+    <t>fu_hyperten</t>
+  </si>
+  <si>
+    <t>fu_hypercho</t>
+  </si>
+  <si>
+    <t>fu_b12def</t>
+  </si>
+  <si>
+    <t>fu_thyroid</t>
+  </si>
+  <si>
+    <t>fu_arthrit</t>
+  </si>
+  <si>
+    <t>fu_arthtype</t>
+  </si>
+  <si>
+    <t>fu_arthtypx</t>
+  </si>
+  <si>
+    <t>fu_arthupex</t>
+  </si>
+  <si>
+    <t>fu_arthloex</t>
+  </si>
+  <si>
+    <t>fu_arthspin</t>
+  </si>
+  <si>
+    <t>fu_arthunk</t>
+  </si>
+  <si>
+    <t>fu_incontu</t>
+  </si>
+  <si>
+    <t>fu_incontf</t>
+  </si>
+  <si>
+    <t>fu_apnea</t>
+  </si>
+  <si>
+    <t>fu_rbd</t>
+  </si>
+  <si>
+    <t>fu_insomn</t>
+  </si>
+  <si>
+    <t>fu_othsleep</t>
+  </si>
+  <si>
+    <t>fu_othsleex</t>
+  </si>
+  <si>
+    <t>fu_alcohol</t>
+  </si>
+  <si>
+    <t>fu_abusothr</t>
+  </si>
+  <si>
+    <t>fu_abusx</t>
+  </si>
+  <si>
+    <t>fu_ptsd</t>
+  </si>
+  <si>
+    <t>fu_bipolar</t>
+  </si>
+  <si>
+    <t>fu_schiz</t>
+  </si>
+  <si>
+    <t>fu_dep2yrs</t>
+  </si>
+  <si>
+    <t>fu_depothr</t>
+  </si>
+  <si>
+    <t>fu_anxiety</t>
+  </si>
+  <si>
+    <t>fu_ocd</t>
+  </si>
+  <si>
+    <t>fu_npsydev</t>
+  </si>
+  <si>
+    <t>fu_psycdis</t>
+  </si>
+  <si>
+    <t>fu_psycdisx</t>
+  </si>
+  <si>
+    <t>fvp_a5_complete</t>
+  </si>
+  <si>
+    <t>fvp_a5</t>
   </si>
 </sst>
 </file>
@@ -3809,7 +4229,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4160,11 +4600,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCC9BF6-0E02-034A-99C2-203518C15656}">
-  <dimension ref="A1:H424"/>
+  <dimension ref="A1:H493"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H373" sqref="H373"/>
+      <pane ySplit="1" topLeftCell="A411" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F432" sqref="F432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14716,7 +15156,7 @@
         <v>1151</v>
       </c>
       <c r="D387" t="b">
-        <f t="shared" ref="D387:D424" si="12">IF(NOT(ISBLANK(C387)),A387=REPLACE(C387,1,3,""),"")</f>
+        <f t="shared" ref="D387:D450" si="12">IF(NOT(ISBLANK(C387)),A387=REPLACE(C387,1,3,""),"")</f>
         <v>1</v>
       </c>
       <c r="E387" t="s">
@@ -15769,23 +16209,1275 @@
         <v>0</v>
       </c>
     </row>
+    <row r="425" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A425" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B425" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C425" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D425" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E425" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="426" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A426" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B426" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C426" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D426" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E426" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="427" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A427" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B427" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C427" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D427" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E427" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="428" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A428" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B428" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C428" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D428" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E428" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="429" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A429" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B429" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C429" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D429" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E429" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="430" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A430" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B430" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C430" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D430" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E430" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="431" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A431" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B431" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C431" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D431" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E431" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="432" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A432" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B432" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C432" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D432" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E432" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="433" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A433" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B433" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C433" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D433" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E433" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="434" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A434" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B434" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C434" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D434" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E434" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="435" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A435" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B435" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C435" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D435" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E435" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="436" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A436" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B436" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C436" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D436" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E436" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="437" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A437" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B437" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C437" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D437" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E437" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="438" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A438" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B438" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C438" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D438" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E438" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="439" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A439" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B439" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C439" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D439" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E439" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="440" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A440" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B440" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C440" t="s">
+        <v>1328</v>
+      </c>
+      <c r="D440" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E440" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="441" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A441" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B441" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C441" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D441" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E441" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="442" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A442" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B442" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C442" t="s">
+        <v>1330</v>
+      </c>
+      <c r="D442" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E442" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="443" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A443" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B443" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C443" t="s">
+        <v>1331</v>
+      </c>
+      <c r="D443" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E443" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="444" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A444" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B444" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C444" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D444" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E444" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="445" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A445" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B445" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C445" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D445" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E445" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="446" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A446" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B446" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C446" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D446" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E446" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A447" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B447" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C447" t="s">
+        <v>1335</v>
+      </c>
+      <c r="D447" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E447" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A448" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B448" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C448" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D448" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E448" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A449" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B449" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C449" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D449" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E449" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="450" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A450" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B450" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C450" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D450" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E450" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="451" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A451" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B451" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C451" t="s">
+        <v>1339</v>
+      </c>
+      <c r="D451" t="b">
+        <f t="shared" ref="D451:D493" si="14">IF(NOT(ISBLANK(C451)),A451=REPLACE(C451,1,3,""),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E451" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="452" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A452" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B452" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C452" t="s">
+        <v>1340</v>
+      </c>
+      <c r="D452" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E452" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="453" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A453" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B453" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C453" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D453" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E453" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A454" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B454" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C454" t="s">
+        <v>1342</v>
+      </c>
+      <c r="D454" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E454" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A455" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B455" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C455" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D455" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E455" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A456" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B456" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C456" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D456" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E456" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A457" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B457" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C457" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D457" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E457" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A458" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B458" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C458" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D458" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E458" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A459" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B459" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C459" t="s">
+        <v>1347</v>
+      </c>
+      <c r="D459" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E459" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="460" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A460" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B460" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C460" t="s">
+        <v>1348</v>
+      </c>
+      <c r="D460" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E460" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A461" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B461" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C461" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D461" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E461" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A462" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B462" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C462" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D462" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E462" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A463" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B463" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C463" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D463" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E463" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A464" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B464" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C464" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D464" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E464" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A465" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B465" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C465" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D465" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E465" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A466" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B466" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C466" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D466" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E466" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="467" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A467" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B467" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C467" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D467" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E467" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="468" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A468" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B468" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C468" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D468" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E468" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="469" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A469" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B469" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C469" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D469" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E469" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="470" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A470" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B470" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C470" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D470" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E470" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="471" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A471" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B471" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C471" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D471" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E471" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A472" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B472" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C472" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D472" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E472" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="473" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A473" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B473" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C473" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D473" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E473" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A474" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B474" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C474" t="s">
+        <v>1362</v>
+      </c>
+      <c r="D474" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E474" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="475" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A475" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B475" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C475" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D475" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E475" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="476" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A476" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B476" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C476" t="s">
+        <v>1364</v>
+      </c>
+      <c r="D476" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E476" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="477" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A477" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B477" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C477" t="s">
+        <v>1365</v>
+      </c>
+      <c r="D477" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E477" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="478" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A478" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B478" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C478" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D478" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E478" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="479" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A479" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B479" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C479" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D479" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E479" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="480" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A480" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B480" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C480" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D480" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E480" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="481" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A481" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B481" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C481" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D481" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E481" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="482" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A482" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B482" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C482" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D482" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E482" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A483" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B483" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C483" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D483" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E483" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A484" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B484" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C484" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D484" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E484" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A485" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B485" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C485" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D485" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E485" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="486" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A486" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B486" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C486" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D486" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E486" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A487" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B487" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C487" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D487" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E487" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A488" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B488" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C488" t="s">
+        <v>1376</v>
+      </c>
+      <c r="D488" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E488" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="489" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A489" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B489" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C489" t="s">
+        <v>1377</v>
+      </c>
+      <c r="D489" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E489" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="490" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A490" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B490" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C490" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D490" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E490" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="491" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A491" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B491" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C491" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D491" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E491" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="492" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A492" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B492" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C492" t="s">
+        <v>1380</v>
+      </c>
+      <c r="D492" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E492" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="493" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A493" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B493" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C493" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D493" t="b">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="E493" t="s">
+        <v>1382</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576 E373 E376 E379 E382 E385 E388 E391 E394 E397 E400 E403 E406 E409 E412 E415 E418 E421 E424">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="E373 E376 E379 E382 E385 E388 E391 E394 E397 E400 E403 E406 E409 E412 E415 E418 E421 D1:D1048576 E424:E425 E428 E431 E434 E437 E440 E443 E446 E449 E452 E455 E458 E461 E464 E467 E470 E473 E476 E479 E482 E485 E488 E491">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E374 E377 E380 E383 E386 E389 E392 E395 E398 E401 E404 E407 E410 E413 E416 E419 E422">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E375 E378 E381 E384 E387 E390 E393 E396 E399 E402 E405 E408 E411 E414 E417 E420 E423">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E426 E429 E432 E435 E438 E441 E444 E447 E450 E453 E456 E459 E462 E465 E468 E471 E474 E477 E480 E483 E486 E489 E492">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E375 E378 E381 E384 E387 E390 E393 E396 E399 E402 E405 E408 E411 E414 E417 E420 E423">
+  <conditionalFormatting sqref="E427 E430 E433 E436 E439 E442 E445 E448 E451 E454 E457 E460 E463 E466 E469 E472 E475 E478 E481 E484 E487 E490 E493">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>

</xml_diff>

<commit_message>
add UDS Forms B1, B2, B3, B4
</commit_message>
<xml_diff>
--- a/WIP__uds3_ift_matches.xlsx
+++ b/WIP__uds3_ift_matches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ldmay/Box Sync/Documents/MADC_Data_Unification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C821789E-2B23-D944-A902-237CFA80B4D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CF58A2-B072-964A-B047-163C2F52C74E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19180" yWindow="460" windowWidth="19200" windowHeight="23540" xr2:uid="{076664BD-647D-FA4F-B94B-D41FA05C105D}"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="12800" windowHeight="24000" xr2:uid="{076664BD-647D-FA4F-B94B-D41FA05C105D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2729" uniqueCount="1383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2843" uniqueCount="1445">
   <si>
     <t>ivp_a1</t>
   </si>
@@ -4179,6 +4179,192 @@
   </si>
   <si>
     <t>fvp_a5</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>ivp_b1</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>bpsys</t>
+  </si>
+  <si>
+    <t>bpdias</t>
+  </si>
+  <si>
+    <t>hrate</t>
+  </si>
+  <si>
+    <t>vision</t>
+  </si>
+  <si>
+    <t>viscorr</t>
+  </si>
+  <si>
+    <t>viswcorr</t>
+  </si>
+  <si>
+    <t>hearing</t>
+  </si>
+  <si>
+    <t>hearaid</t>
+  </si>
+  <si>
+    <t>hearwaid</t>
+  </si>
+  <si>
+    <t>ivp_b1_complete</t>
+  </si>
+  <si>
+    <t>fu_height</t>
+  </si>
+  <si>
+    <t>fu_weight</t>
+  </si>
+  <si>
+    <t>fu_bpsys</t>
+  </si>
+  <si>
+    <t>fu_bpdias</t>
+  </si>
+  <si>
+    <t>fu_hrate</t>
+  </si>
+  <si>
+    <t>fu_vision</t>
+  </si>
+  <si>
+    <t>fu_viscorr</t>
+  </si>
+  <si>
+    <t>fu_viswcorr</t>
+  </si>
+  <si>
+    <t>fu_hearing</t>
+  </si>
+  <si>
+    <t>fu_hearaid</t>
+  </si>
+  <si>
+    <t>fu_hearwaid</t>
+  </si>
+  <si>
+    <t>fvp_b1_complete</t>
+  </si>
+  <si>
+    <t>fvp_b1</t>
+  </si>
+  <si>
+    <t>memory</t>
+  </si>
+  <si>
+    <t>ivp_b4</t>
+  </si>
+  <si>
+    <t>orient</t>
+  </si>
+  <si>
+    <t>judgment</t>
+  </si>
+  <si>
+    <t>commun</t>
+  </si>
+  <si>
+    <t>homehobb</t>
+  </si>
+  <si>
+    <t>perscare</t>
+  </si>
+  <si>
+    <t>cdrsum</t>
+  </si>
+  <si>
+    <t>cdrglob</t>
+  </si>
+  <si>
+    <t>comport</t>
+  </si>
+  <si>
+    <t>cdrlang</t>
+  </si>
+  <si>
+    <t>ivp_b4_complete</t>
+  </si>
+  <si>
+    <t>fu_memory</t>
+  </si>
+  <si>
+    <t>fu_orient</t>
+  </si>
+  <si>
+    <t>fu_judgment</t>
+  </si>
+  <si>
+    <t>fu_commun</t>
+  </si>
+  <si>
+    <t>fu_homehobb</t>
+  </si>
+  <si>
+    <t>fu_perscare</t>
+  </si>
+  <si>
+    <t>fu_cdrsum</t>
+  </si>
+  <si>
+    <t>fu_cdrglob</t>
+  </si>
+  <si>
+    <t>fu_comport</t>
+  </si>
+  <si>
+    <t>fu_cdrlang</t>
+  </si>
+  <si>
+    <t>fvp_b4_complete</t>
+  </si>
+  <si>
+    <t>fvp_b4</t>
+  </si>
+  <si>
+    <t>tele_memory</t>
+  </si>
+  <si>
+    <t>tele_orient</t>
+  </si>
+  <si>
+    <t>tele_judgment</t>
+  </si>
+  <si>
+    <t>tele_commun</t>
+  </si>
+  <si>
+    <t>tele_homehobb</t>
+  </si>
+  <si>
+    <t>tele_perscare</t>
+  </si>
+  <si>
+    <t>tele_cdrsum</t>
+  </si>
+  <si>
+    <t>tele_cdrglob</t>
+  </si>
+  <si>
+    <t>tele_comport</t>
+  </si>
+  <si>
+    <t>tele_cdrlang</t>
+  </si>
+  <si>
+    <t>tvp_b4_complete</t>
+  </si>
+  <si>
+    <t>tvp_b4</t>
   </si>
 </sst>
 </file>
@@ -4229,7 +4415,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4600,11 +4826,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCC9BF6-0E02-034A-99C2-203518C15656}">
-  <dimension ref="A1:H493"/>
+  <dimension ref="A1:H516"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A411" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F432" sqref="F432"/>
+      <pane ySplit="1" topLeftCell="A473" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A516" sqref="A516"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15169,7 +15395,7 @@
         <v>1242</v>
       </c>
       <c r="H387" t="b">
-        <f t="shared" ref="H387:H424" si="13">IF(NOT(ISBLANK(F387)),A387=REPLACE(F387,1,5,""),"")</f>
+        <f t="shared" ref="H387:H450" si="13">IF(NOT(ISBLANK(F387)),A387=REPLACE(F387,1,5,""),"")</f>
         <v>1</v>
       </c>
     </row>
@@ -16226,6 +16452,10 @@
       <c r="E425" t="s">
         <v>1382</v>
       </c>
+      <c r="H425" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
     </row>
     <row r="426" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
@@ -16244,6 +16474,10 @@
       <c r="E426" t="s">
         <v>1382</v>
       </c>
+      <c r="H426" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
     </row>
     <row r="427" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
@@ -16262,6 +16496,10 @@
       <c r="E427" t="s">
         <v>1382</v>
       </c>
+      <c r="H427" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
     </row>
     <row r="428" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
@@ -16280,6 +16518,10 @@
       <c r="E428" t="s">
         <v>1382</v>
       </c>
+      <c r="H428" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
     </row>
     <row r="429" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
@@ -16298,6 +16540,10 @@
       <c r="E429" t="s">
         <v>1382</v>
       </c>
+      <c r="H429" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
     </row>
     <row r="430" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
@@ -16316,6 +16562,10 @@
       <c r="E430" t="s">
         <v>1382</v>
       </c>
+      <c r="H430" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
     </row>
     <row r="431" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
@@ -16334,6 +16584,10 @@
       <c r="E431" t="s">
         <v>1382</v>
       </c>
+      <c r="H431" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
     </row>
     <row r="432" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
@@ -16352,8 +16606,12 @@
       <c r="E432" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H432" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="433" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>1251</v>
       </c>
@@ -16370,8 +16628,12 @@
       <c r="E433" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H433" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="434" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>1252</v>
       </c>
@@ -16388,8 +16650,12 @@
       <c r="E434" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H434" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="435" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>1253</v>
       </c>
@@ -16406,8 +16672,12 @@
       <c r="E435" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H435" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="436" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>1254</v>
       </c>
@@ -16424,8 +16694,12 @@
       <c r="E436" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H436" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="437" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>1255</v>
       </c>
@@ -16442,8 +16716,12 @@
       <c r="E437" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H437" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="438" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>1256</v>
       </c>
@@ -16460,8 +16738,12 @@
       <c r="E438" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H438" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="439" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>1257</v>
       </c>
@@ -16478,8 +16760,12 @@
       <c r="E439" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H439" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="440" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>1258</v>
       </c>
@@ -16496,8 +16782,12 @@
       <c r="E440" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H440" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="441" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>1259</v>
       </c>
@@ -16514,8 +16804,12 @@
       <c r="E441" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H441" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="442" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
         <v>1260</v>
       </c>
@@ -16532,8 +16826,12 @@
       <c r="E442" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H442" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="443" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
         <v>1261</v>
       </c>
@@ -16550,8 +16848,12 @@
       <c r="E443" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H443" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="444" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
         <v>1262</v>
       </c>
@@ -16568,8 +16870,12 @@
       <c r="E444" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H444" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="445" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
         <v>1263</v>
       </c>
@@ -16586,8 +16892,12 @@
       <c r="E445" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H445" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="446" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
         <v>1264</v>
       </c>
@@ -16604,8 +16914,12 @@
       <c r="E446" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H446" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="447" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>1265</v>
       </c>
@@ -16622,8 +16936,12 @@
       <c r="E447" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H447" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="448" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
         <v>1266</v>
       </c>
@@ -16640,8 +16958,12 @@
       <c r="E448" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H448" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="449" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>1267</v>
       </c>
@@ -16658,8 +16980,12 @@
       <c r="E449" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H449" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="450" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>1268</v>
       </c>
@@ -16676,8 +17002,12 @@
       <c r="E450" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H450" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="451" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>1269</v>
       </c>
@@ -16688,14 +17018,18 @@
         <v>1339</v>
       </c>
       <c r="D451" t="b">
-        <f t="shared" ref="D451:D493" si="14">IF(NOT(ISBLANK(C451)),A451=REPLACE(C451,1,3,""),"")</f>
+        <f t="shared" ref="D451:D514" si="14">IF(NOT(ISBLANK(C451)),A451=REPLACE(C451,1,3,""),"")</f>
         <v>1</v>
       </c>
       <c r="E451" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H451" t="str">
+        <f t="shared" ref="H451:H514" si="15">IF(NOT(ISBLANK(F451)),A451=REPLACE(F451,1,5,""),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="452" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
         <v>1270</v>
       </c>
@@ -16712,8 +17046,12 @@
       <c r="E452" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H452" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="453" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>1271</v>
       </c>
@@ -16730,8 +17068,12 @@
       <c r="E453" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H453" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="454" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
         <v>1272</v>
       </c>
@@ -16748,8 +17090,12 @@
       <c r="E454" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H454" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="455" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
         <v>1273</v>
       </c>
@@ -16766,8 +17112,12 @@
       <c r="E455" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H455" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="456" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
         <v>1274</v>
       </c>
@@ -16784,8 +17134,12 @@
       <c r="E456" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H456" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="457" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>1275</v>
       </c>
@@ -16802,8 +17156,12 @@
       <c r="E457" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H457" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="458" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
         <v>1276</v>
       </c>
@@ -16820,8 +17178,12 @@
       <c r="E458" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H458" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="459" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
         <v>1277</v>
       </c>
@@ -16838,8 +17200,12 @@
       <c r="E459" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H459" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="460" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
         <v>1278</v>
       </c>
@@ -16856,8 +17222,12 @@
       <c r="E460" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H460" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="461" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
         <v>1279</v>
       </c>
@@ -16874,8 +17244,12 @@
       <c r="E461" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H461" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="462" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
         <v>1280</v>
       </c>
@@ -16892,8 +17266,12 @@
       <c r="E462" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H462" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="463" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
         <v>1281</v>
       </c>
@@ -16910,8 +17288,12 @@
       <c r="E463" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H463" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="464" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
         <v>1282</v>
       </c>
@@ -16928,8 +17310,12 @@
       <c r="E464" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H464" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="465" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>1283</v>
       </c>
@@ -16946,8 +17332,12 @@
       <c r="E465" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H465" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="466" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>1284</v>
       </c>
@@ -16964,8 +17354,12 @@
       <c r="E466" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H466" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="467" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
         <v>1285</v>
       </c>
@@ -16982,8 +17376,12 @@
       <c r="E467" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H467" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="468" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>1286</v>
       </c>
@@ -17000,8 +17398,12 @@
       <c r="E468" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H468" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="469" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
         <v>1287</v>
       </c>
@@ -17018,8 +17420,12 @@
       <c r="E469" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H469" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="470" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
         <v>1288</v>
       </c>
@@ -17036,8 +17442,12 @@
       <c r="E470" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H470" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="471" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
         <v>1289</v>
       </c>
@@ -17054,8 +17464,12 @@
       <c r="E471" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H471" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="472" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>1290</v>
       </c>
@@ -17072,8 +17486,12 @@
       <c r="E472" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H472" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="473" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
         <v>1291</v>
       </c>
@@ -17090,8 +17508,12 @@
       <c r="E473" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H473" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="474" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>1292</v>
       </c>
@@ -17108,8 +17530,12 @@
       <c r="E474" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H474" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="475" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
         <v>1293</v>
       </c>
@@ -17126,8 +17552,12 @@
       <c r="E475" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H475" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="476" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
         <v>1294</v>
       </c>
@@ -17144,8 +17574,12 @@
       <c r="E476" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H476" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="477" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
         <v>1295</v>
       </c>
@@ -17162,8 +17596,12 @@
       <c r="E477" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H477" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="478" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
         <v>1296</v>
       </c>
@@ -17180,8 +17618,12 @@
       <c r="E478" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H478" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="479" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
         <v>1297</v>
       </c>
@@ -17198,8 +17640,12 @@
       <c r="E479" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H479" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="480" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
         <v>1298</v>
       </c>
@@ -17216,8 +17662,12 @@
       <c r="E480" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="481" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H480" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="481" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
         <v>1299</v>
       </c>
@@ -17234,8 +17684,12 @@
       <c r="E481" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="482" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H481" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="482" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
         <v>1300</v>
       </c>
@@ -17252,8 +17706,12 @@
       <c r="E482" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="483" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H482" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="483" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
         <v>1301</v>
       </c>
@@ -17270,8 +17728,12 @@
       <c r="E483" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="484" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H483" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="484" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
         <v>1302</v>
       </c>
@@ -17288,8 +17750,12 @@
       <c r="E484" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="485" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H484" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="485" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
         <v>1303</v>
       </c>
@@ -17306,8 +17772,12 @@
       <c r="E485" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="486" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H485" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="486" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
         <v>1304</v>
       </c>
@@ -17324,8 +17794,12 @@
       <c r="E486" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="487" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H486" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="487" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
         <v>1305</v>
       </c>
@@ -17342,8 +17816,12 @@
       <c r="E487" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="488" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H487" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="488" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
         <v>1306</v>
       </c>
@@ -17360,8 +17838,12 @@
       <c r="E488" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="489" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H488" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="489" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
         <v>1307</v>
       </c>
@@ -17378,8 +17860,12 @@
       <c r="E489" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="490" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H489" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="490" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
         <v>1308</v>
       </c>
@@ -17396,8 +17882,12 @@
       <c r="E490" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="491" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H490" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="491" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
         <v>1309</v>
       </c>
@@ -17414,8 +17904,12 @@
       <c r="E491" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="492" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H491" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="492" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
         <v>1310</v>
       </c>
@@ -17432,8 +17926,12 @@
       <c r="E492" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="493" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H492" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="493" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
         <v>1311</v>
       </c>
@@ -17450,34 +17948,630 @@
       <c r="E493" t="s">
         <v>1382</v>
       </c>
+      <c r="H493" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="494" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A494" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B494" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C494" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D494" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E494" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H494" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="495" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A495" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B495" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C495" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D495" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E495" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H495" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="496" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A496" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B496" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C496" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D496" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E496" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H496" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A497" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B497" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C497" t="s">
+        <v>1399</v>
+      </c>
+      <c r="D497" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E497" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H497" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="498" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A498" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B498" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C498" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D498" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E498" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H498" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="499" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A499" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B499" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C499" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D499" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E499" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H499" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="500" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A500" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B500" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C500" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D500" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E500" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H500" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="501" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A501" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B501" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C501" t="s">
+        <v>1403</v>
+      </c>
+      <c r="D501" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E501" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H501" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="502" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A502" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B502" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C502" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D502" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E502" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H502" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="503" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A503" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B503" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C503" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D503" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E503" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H503" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="504" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A504" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B504" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C504" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D504" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E504" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H504" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="505" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A505" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B505" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C505" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D505" t="b">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="E505" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H505" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="506" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A506" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B506" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C506" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D506" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E506" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F506" t="s">
+        <v>1433</v>
+      </c>
+      <c r="G506" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H506" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="507" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A507" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B507" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C507" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D507" t="b">
+        <f>IF(NOT(ISBLANK(C507)),A507=REPLACE(C507,1,3,""),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E507" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F507" t="s">
+        <v>1434</v>
+      </c>
+      <c r="G507" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H507" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="508" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A508" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B508" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C508" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D508" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E508" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F508" t="s">
+        <v>1435</v>
+      </c>
+      <c r="G508" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H508" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="509" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A509" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B509" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C509" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D509" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E509" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F509" t="s">
+        <v>1436</v>
+      </c>
+      <c r="G509" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H509" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="510" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A510" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B510" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C510" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D510" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E510" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F510" t="s">
+        <v>1437</v>
+      </c>
+      <c r="G510" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H510" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="511" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A511" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B511" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C511" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D511" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E511" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F511" t="s">
+        <v>1438</v>
+      </c>
+      <c r="G511" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H511" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="512" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A512" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B512" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C512" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D512" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E512" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F512" t="s">
+        <v>1439</v>
+      </c>
+      <c r="G512" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H512" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A513" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B513" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C513" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D513" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E513" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F513" t="s">
+        <v>1440</v>
+      </c>
+      <c r="G513" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H513" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A514" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B514" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C514" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D514" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E514" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F514" t="s">
+        <v>1441</v>
+      </c>
+      <c r="G514" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H514" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A515" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B515" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C515" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D515" t="b">
+        <f t="shared" ref="D515:D516" si="16">IF(NOT(ISBLANK(C515)),A515=REPLACE(C515,1,3,""),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E515" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F515" t="s">
+        <v>1442</v>
+      </c>
+      <c r="G515" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H515" t="b">
+        <f t="shared" ref="H515:H516" si="17">IF(NOT(ISBLANK(F515)),A515=REPLACE(F515,1,5,""),"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A516" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B516" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C516" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D516" t="b">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="E516" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F516" t="s">
+        <v>1443</v>
+      </c>
+      <c r="G516" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H516" t="b">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E373 E376 E379 E382 E385 E388 E391 E394 E397 E400 E403 E406 E409 E412 E415 E418 E421 D1:D1048576 E424:E425 E428 E431 E434 E437 E440 E443 E446 E449 E452 E455 E458 E461 E464 E467 E470 E473 E476 E479 E482 E485 E488 E491">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+  <conditionalFormatting sqref="E373 E376 E379 E382 E385 E388 E391 E394 E397 E400 E403 E406 E409 E412 E415 E418 E421 E424:E425 E428 E431 E434 E437 E440 E443 E446 E449 E452 E455 E458 E461 E464 E467 E470 E473 E476 E479 E482 E485 E488 E491 E494 E497 E500 E503 D1:D1048576 E506 E510 E514 H1:H1048576">
+    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
+  <conditionalFormatting sqref="E374 E377 E380 E383 E386 E389 E392 E395 E398 E401 E404 E407 E410 E413 E416 E419 E422">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E375 E378 E381 E384 E387 E390 E393 E396 E399 E402 E405 E408 E411 E414 E417 E420 E423">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E426 E429 E432 E435 E438 E441 E444 E447 E450 E453 E456 E459 E462 E465 E468 E471 E474 E477 E480 E483 E486 E489 E492">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E427 E430 E433 E436 E439 E442 E445 E448 E451 E454 E457 E460 E463 E466 E469 E472 E475 E478 E481 E484 E487 E490 E493">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E495 E498 E501 E504">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E374 E377 E380 E383 E386 E389 E392 E395 E398 E401 E404 E407 E410 E413 E416 E419 E422">
+  <conditionalFormatting sqref="E496 E499 E502 E505">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E375 E378 E381 E384 E387 E390 E393 E396 E399 E402 E405 E408 E411 E414 E417 E420 E423">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="E507 E511 E515">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E426 E429 E432 E435 E438 E441 E444 E447 E450 E453 E456 E459 E462 E465 E468 E471 E474 E477 E480 E483 E486 E489 E492">
+  <conditionalFormatting sqref="E508 E512 E516">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E427 E430 E433 E436 E439 E442 E445 E448 E451 E454 E457 E460 E463 E466 E469 E472 E475 E478 E481 E484 E487 E490 E493">
+  <conditionalFormatting sqref="E509 E513">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>

</xml_diff>